<commit_message>
Wersja 1.1 PCB sekwencera - dodany status LED
</commit_message>
<xml_diff>
--- a/5 step sequencer/Outputs/BOM/5_step_seq_BOM.xlsx
+++ b/5 step sequencer/Outputs/BOM/5_step_seq_BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jakub\Desktop\Eurorack-project\5 step sequencer\Outputs\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CC678DF-368E-4A9D-9149-972F87FA6DDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FA6206C1-EB3F-4010-A245-2FB7CF3A1395}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5010" yWindow="3705" windowWidth="28800" windowHeight="15435" xr2:uid="{055E1850-8932-4892-B348-441A755D2E31}"/>
+    <workbookView xWindow="5010" yWindow="3705" windowWidth="28800" windowHeight="15435" xr2:uid="{74F7E387-367E-48C7-9582-ECDC9CF48550}"/>
   </bookViews>
   <sheets>
     <sheet name="5_step_seq_BOM" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="72">
   <si>
     <t>Quantity</t>
   </si>
@@ -125,6 +125,12 @@
     <t>J6</t>
   </si>
   <si>
+    <t>LED SMD</t>
+  </si>
+  <si>
+    <t>D23</t>
+  </si>
+  <si>
     <t>LED THT</t>
   </si>
   <si>
@@ -144,6 +150,15 @@
   </si>
   <si>
     <t>P2, P3, P4, P5, P8</t>
+  </si>
+  <si>
+    <t>Resistor SMD 0805</t>
+  </si>
+  <si>
+    <t>10k</t>
+  </si>
+  <si>
+    <t>R30</t>
   </si>
   <si>
     <t>Resistor THT</t>
@@ -297,21 +312,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -645,18 +651,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{004BB201-6EE6-45C5-8E12-65274E88A0A5}">
-  <dimension ref="A1:E28"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB1B6696-8012-4AD2-985E-E60BAD652079}">
+  <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="19.7109375" customWidth="1"/>
     <col min="3" max="4" width="16.5703125" customWidth="1"/>
-    <col min="5" max="5" width="19.7109375" style="7" customWidth="1"/>
+    <col min="5" max="5" width="19.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -672,7 +676,7 @@
       <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
     </row>
@@ -685,7 +689,7 @@
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -698,11 +702,11 @@
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>6</v>
       </c>
@@ -711,7 +715,7 @@
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="2" t="s">
         <v>10</v>
       </c>
     </row>
@@ -726,7 +730,7 @@
         <v>12</v>
       </c>
       <c r="D5" s="1"/>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="2" t="s">
         <v>13</v>
       </c>
     </row>
@@ -741,7 +745,7 @@
         <v>15</v>
       </c>
       <c r="D6" s="1"/>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="2" t="s">
         <v>16</v>
       </c>
     </row>
@@ -756,7 +760,7 @@
         <v>17</v>
       </c>
       <c r="D7" s="1"/>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="2" t="s">
         <v>18</v>
       </c>
     </row>
@@ -771,7 +775,7 @@
         <v>19</v>
       </c>
       <c r="D8" s="1"/>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="2" t="s">
         <v>20</v>
       </c>
     </row>
@@ -784,11 +788,11 @@
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
-      <c r="E9" s="6" t="s">
+      <c r="E9" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>15</v>
       </c>
@@ -799,7 +803,7 @@
       <c r="D10" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="E10" s="2" t="s">
         <v>25</v>
       </c>
     </row>
@@ -812,20 +816,20 @@
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
-      <c r="E11" s="6" t="s">
+      <c r="E11" s="2" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>28</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
-      <c r="E12" s="6" t="s">
+      <c r="E12" s="2" t="s">
         <v>29</v>
       </c>
     </row>
@@ -838,7 +842,7 @@
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
-      <c r="E13" s="6" t="s">
+      <c r="E13" s="2" t="s">
         <v>31</v>
       </c>
     </row>
@@ -849,27 +853,25 @@
       <c r="B14" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="D14" s="1"/>
-      <c r="E14" s="6" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B15" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="D15" s="1"/>
+      <c r="E15" s="2" t="s">
         <v>36</v>
-      </c>
-      <c r="D15" s="1"/>
-      <c r="E15" s="6" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -877,13 +879,13 @@
         <v>1</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>38</v>
       </c>
       <c r="D16" s="1"/>
-      <c r="E16" s="6" t="s">
+      <c r="E16" s="2" t="s">
         <v>39</v>
       </c>
     </row>
@@ -892,14 +894,14 @@
         <v>1</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D17" s="1"/>
-      <c r="E17" s="6" t="s">
-        <v>41</v>
+      <c r="E17" s="2" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -907,14 +909,14 @@
         <v>1</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D18" s="1"/>
-      <c r="E18" s="6" t="s">
-        <v>43</v>
+      <c r="E18" s="2" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -922,14 +924,14 @@
         <v>1</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D19" s="1"/>
-      <c r="E19" s="6" t="s">
-        <v>45</v>
+      <c r="E19" s="2" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -937,14 +939,14 @@
         <v>1</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D20" s="1"/>
-      <c r="E20" s="6" t="s">
-        <v>47</v>
+      <c r="E20" s="2" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -952,86 +954,88 @@
         <v>1</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D21" s="1"/>
-      <c r="E21" s="6" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="E21" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D22" s="1"/>
-      <c r="E22" s="6" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="E22" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D23" s="1"/>
-      <c r="E23" s="6" t="s">
-        <v>53</v>
+      <c r="E23" s="2" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C24" s="1"/>
-      <c r="D24" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="E24" s="6" t="s">
+      <c r="D24" s="1"/>
+      <c r="E24" s="2" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="B25" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C25" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C25" s="1"/>
       <c r="D25" s="1"/>
-      <c r="E25" s="6" t="s">
+      <c r="E25" s="2" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C26" s="1"/>
+      <c r="D26" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="D26" s="1"/>
-      <c r="E26" s="6" t="s">
+      <c r="E26" s="2" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1040,13 +1044,11 @@
         <v>1</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C27" s="2" t="s">
         <v>62</v>
       </c>
+      <c r="C27" s="1"/>
       <c r="D27" s="1"/>
-      <c r="E27" s="6" t="s">
+      <c r="E27" s="2" t="s">
         <v>63</v>
       </c>
     </row>
@@ -1061,8 +1063,38 @@
         <v>65</v>
       </c>
       <c r="D28" s="1"/>
-      <c r="E28" s="6" t="s">
+      <c r="E28" s="2" t="s">
         <v>66</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>1</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D29" s="1"/>
+      <c r="E29" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>1</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D30" s="1"/>
+      <c r="E30" s="2" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>